<commit_message>
Currently does not account for split schools. Treats all duplicate schools as separate schools.
</commit_message>
<xml_diff>
--- a/LBDL/testInput.xlsx
+++ b/LBDL/testInput.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="120" windowWidth="37400" windowHeight="13540"/>
+    <workbookView xWindow="144" yWindow="120" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="172">
   <si>
     <t>St. Patrick Catholic School</t>
   </si>
@@ -258,9 +258,6 @@
     <t>Can't wait - this is one of the highlights of the year for my students and for me! My students loop with me from 7th to 8th grade and they are thrilled that one of those years includes this trip to CalPoly!!!</t>
   </si>
   <si>
-    <t>Atascadero fine arts academy</t>
-  </si>
-  <si>
     <t>3/25 to 3/31</t>
   </si>
   <si>
@@ -303,9 +300,6 @@
     <t xml:space="preserve">Please take us!!! We love the Learn By Doing Lab and the Cal Poly campus!!!! </t>
   </si>
   <si>
-    <t>Fesler Junior High</t>
-  </si>
-  <si>
     <t>March 28 - April 1, 2015</t>
   </si>
   <si>
@@ -313,9 +307,6 @@
   </si>
   <si>
     <t>San Benito Road Elementary</t>
-  </si>
-  <si>
-    <t>atascaero fine arts academy</t>
   </si>
   <si>
     <t>Creston Elementary School</t>
@@ -548,6 +539,12 @@
     <t>If needed, I am willing
 to split my class over
 two (or more) days.</t>
+  </si>
+  <si>
+    <t>Atascadero Fine Arts Academy</t>
+  </si>
+  <si>
+    <t>Atascaero Fine Arts Academy</t>
   </si>
 </sst>
 </file>
@@ -1273,137 +1270,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1692,7 +1559,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1702,148 +1569,148 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="36" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="203.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="203.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="2" customFormat="1" ht="42">
+    <row r="1" spans="1:39" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y1" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC1" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="AD1" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="AE1" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="AF1" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="AG1" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH1" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="AI1" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="AJ1" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="AK1" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="AL1" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="U1" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="V1" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="W1" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="X1" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="Z1" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="AA1" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="AB1" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="AD1" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="AE1" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="AF1" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="AG1" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="AH1" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="AI1" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="AJ1" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="AK1" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="AL1" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>162</v>
-      </c>
     </row>
-    <row r="2" spans="1:39">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1854,7 +1721,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="1">
@@ -1958,7 +1825,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -1966,10 +1833,10 @@
         <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="1">
@@ -2075,7 +1942,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1.2</v>
       </c>
@@ -2083,10 +1950,10 @@
         <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="1">
@@ -2187,7 +2054,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:39" s="4" customFormat="1">
+    <row r="5" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1.3</v>
       </c>
@@ -2195,10 +2062,10 @@
         <v>52</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E5" s="14">
         <v>104</v>
@@ -2304,7 +2171,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:39" s="4" customFormat="1">
+    <row r="6" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1.3</v>
       </c>
@@ -2312,10 +2179,10 @@
         <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="1">
@@ -2419,7 +2286,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:39" s="4" customFormat="1">
+    <row r="7" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1.4</v>
       </c>
@@ -2427,10 +2294,10 @@
         <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E7" s="14">
         <v>135</v>
@@ -2476,7 +2343,7 @@
         <v>0</v>
       </c>
       <c r="T7" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="U7" s="15">
         <v>1</v>
@@ -2536,7 +2403,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:39" s="4" customFormat="1">
+    <row r="8" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1.4</v>
       </c>
@@ -2544,10 +2411,10 @@
         <v>60</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="1">
@@ -2591,7 +2458,7 @@
         <v>0</v>
       </c>
       <c r="T8" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="U8" s="15">
         <v>1</v>
@@ -2651,7 +2518,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:39" s="4" customFormat="1">
+    <row r="9" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1.5</v>
       </c>
@@ -2662,7 +2529,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="1">
@@ -2714,7 +2581,7 @@
         <v>1</v>
       </c>
       <c r="V9" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="W9" s="15">
         <v>1</v>
@@ -2744,13 +2611,13 @@
         <v>1</v>
       </c>
       <c r="AF9" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AG9" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AH9" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AI9" s="15">
         <v>1</v>
@@ -2766,7 +2633,7 @@
       </c>
       <c r="AM9" s="1"/>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1.6</v>
       </c>
@@ -2774,10 +2641,10 @@
         <v>72</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="8">
@@ -2880,10 +2747,10 @@
         <v>42531</v>
       </c>
       <c r="AM10" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1.7</v>
       </c>
@@ -2891,10 +2758,10 @@
         <v>76</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="1">
@@ -2998,7 +2865,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1.9</v>
       </c>
@@ -3009,7 +2876,7 @@
         <v>15</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="1">
@@ -3067,7 +2934,7 @@
         <v>0</v>
       </c>
       <c r="X12" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Y12" s="15">
         <v>1</v>
@@ -3115,7 +2982,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -3126,7 +2993,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="1">
@@ -3230,18 +3097,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1">
@@ -3338,27 +3205,27 @@
         <v>1</v>
       </c>
       <c r="AK14" s="15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AL14" s="15">
         <v>42164</v>
       </c>
       <c r="AM14" s="15" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>5</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E15" s="20">
         <v>130</v>
@@ -3374,64 +3241,64 @@
         <v>65</v>
       </c>
       <c r="J15" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K15" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L15" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M15" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="N15" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="O15" s="21">
         <v>1</v>
       </c>
       <c r="P15" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Q15" s="21">
         <v>1</v>
       </c>
       <c r="R15" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="S15" s="21">
         <v>1</v>
       </c>
       <c r="T15" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="U15" s="21">
         <v>1</v>
       </c>
       <c r="V15" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="W15" s="21">
         <v>1</v>
       </c>
       <c r="X15" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Y15" s="21">
         <v>1</v>
       </c>
       <c r="Z15" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AA15" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AB15" s="21">
         <v>1</v>
       </c>
       <c r="AC15" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AD15" s="21">
         <v>1</v>
@@ -3443,16 +3310,16 @@
         <v>1</v>
       </c>
       <c r="AG15" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AH15" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AI15" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AJ15" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AK15" s="8" t="s">
         <v>44</v>
@@ -3461,21 +3328,21 @@
         <v>42177</v>
       </c>
       <c r="AM15" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>5</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="8">
@@ -3489,64 +3356,64 @@
         <v>65</v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K16" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L16" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M16" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="N16" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="O16" s="21">
         <v>1</v>
       </c>
       <c r="P16" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Q16" s="21">
         <v>1</v>
       </c>
       <c r="R16" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="S16" s="21">
         <v>1</v>
       </c>
       <c r="T16" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="U16" s="21">
         <v>1</v>
       </c>
       <c r="V16" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="W16" s="21">
         <v>1</v>
       </c>
       <c r="X16" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Y16" s="21">
         <v>1</v>
       </c>
       <c r="Z16" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AA16" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AB16" s="21">
         <v>1</v>
       </c>
       <c r="AC16" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AD16" s="21">
         <v>1</v>
@@ -3558,16 +3425,16 @@
         <v>1</v>
       </c>
       <c r="AG16" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AH16" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AI16" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AJ16" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AK16" s="8" t="s">
         <v>44</v>
@@ -3576,10 +3443,10 @@
         <v>42177</v>
       </c>
       <c r="AM16" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>6</v>
       </c>
@@ -3590,7 +3457,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E17" s="14">
         <v>128</v>
@@ -3694,7 +3561,7 @@
       </c>
       <c r="AM17" s="1"/>
     </row>
-    <row r="18" spans="1:39">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>6</v>
       </c>
@@ -3705,7 +3572,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="1">
@@ -3807,7 +3674,7 @@
       </c>
       <c r="AM18" s="1"/>
     </row>
-    <row r="19" spans="1:39">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>7</v>
       </c>
@@ -3815,10 +3682,10 @@
         <v>73</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="1">
@@ -3924,18 +3791,18 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:39">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>8</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="5">
@@ -4038,10 +3905,10 @@
         <v>42164</v>
       </c>
       <c r="AM20" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:39">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>9</v>
       </c>
@@ -4052,7 +3919,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E21" s="14">
         <v>87</v>
@@ -4158,18 +4025,18 @@
       </c>
       <c r="AM21" s="15"/>
     </row>
-    <row r="22" spans="1:39">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="1">
@@ -4268,7 +4135,7 @@
       </c>
       <c r="AM22" s="1"/>
     </row>
-    <row r="23" spans="1:39">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>12</v>
       </c>
@@ -4279,7 +4146,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E23" s="14">
         <v>140</v>
@@ -4385,7 +4252,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:39">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>12</v>
       </c>
@@ -4396,7 +4263,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="1">
@@ -4500,18 +4367,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:39">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>13</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E25" s="14"/>
       <c r="F25" s="1">
@@ -4606,27 +4473,27 @@
         <v>0</v>
       </c>
       <c r="AK25" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AL25" s="16">
         <v>42531</v>
       </c>
       <c r="AM25" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:39">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>14</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E26" s="17">
         <v>150</v>
@@ -4642,13 +4509,13 @@
         <v>34</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K26" s="18">
         <v>1</v>
       </c>
       <c r="L26" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M26" s="18">
         <v>1</v>
@@ -4660,19 +4527,19 @@
         <v>1</v>
       </c>
       <c r="P26" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Q26" s="18">
         <v>1</v>
       </c>
       <c r="R26" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="S26" s="18">
         <v>1</v>
       </c>
       <c r="T26" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="U26" s="18">
         <v>1</v>
@@ -4690,16 +4557,16 @@
         <v>1</v>
       </c>
       <c r="Z26" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AA26" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AB26" s="18">
         <v>1</v>
       </c>
       <c r="AC26" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AD26" s="18">
         <v>1</v>
@@ -4711,13 +4578,13 @@
         <v>1</v>
       </c>
       <c r="AG26" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AH26" s="18">
         <v>1</v>
       </c>
       <c r="AI26" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AJ26" s="18">
         <v>1</v>
@@ -4730,18 +4597,18 @@
       </c>
       <c r="AM26" s="5"/>
     </row>
-    <row r="27" spans="1:39">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>14</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="5">
@@ -4755,13 +4622,13 @@
         <v>34</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K27" s="18">
         <v>1</v>
       </c>
       <c r="L27" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M27" s="18">
         <v>1</v>
@@ -4773,19 +4640,19 @@
         <v>1</v>
       </c>
       <c r="P27" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Q27" s="18">
         <v>1</v>
       </c>
       <c r="R27" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="S27" s="18">
         <v>1</v>
       </c>
       <c r="T27" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="U27" s="18">
         <v>1</v>
@@ -4803,16 +4670,16 @@
         <v>1</v>
       </c>
       <c r="Z27" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AA27" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AB27" s="18">
         <v>1</v>
       </c>
       <c r="AC27" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AD27" s="18">
         <v>1</v>
@@ -4824,13 +4691,13 @@
         <v>1</v>
       </c>
       <c r="AG27" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AH27" s="18">
         <v>1</v>
       </c>
       <c r="AI27" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AJ27" s="18">
         <v>1</v>
@@ -4843,18 +4710,18 @@
       </c>
       <c r="AM27" s="5"/>
     </row>
-    <row r="28" spans="1:39">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>15</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>79</v>
+        <v>170</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E28" s="17">
         <v>48</v>
@@ -4870,64 +4737,64 @@
         <v>24</v>
       </c>
       <c r="J28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="N28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="O28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="P28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Q28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="R28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="S28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="T28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="U28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="V28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="W28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="X28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Y28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Z28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AA28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AB28" s="18">
         <v>1</v>
       </c>
       <c r="AC28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AD28" s="18">
         <v>1</v>
@@ -4939,37 +4806,37 @@
         <v>1</v>
       </c>
       <c r="AG28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AH28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AI28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AJ28" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AK28" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AL28" s="19">
         <v>42529</v>
       </c>
       <c r="AM28" s="5"/>
     </row>
-    <row r="29" spans="1:39">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>16</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="1">
@@ -5060,20 +4927,20 @@
         <v>1</v>
       </c>
       <c r="AI29" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AJ29" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AK29" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AL29" s="16">
         <v>42531</v>
       </c>
       <c r="AM29" s="1"/>
     </row>
-    <row r="30" spans="1:39" s="4" customFormat="1">
+    <row r="30" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>17</v>
       </c>
@@ -5084,7 +4951,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="1">
@@ -5185,10 +5052,10 @@
         <v>42163</v>
       </c>
       <c r="AM30" s="15" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
-    <row r="31" spans="1:39" s="4" customFormat="1">
+    <row r="31" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>18</v>
       </c>
@@ -5199,7 +5066,7 @@
         <v>2</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="5">
@@ -5228,7 +5095,7 @@
         <v>1</v>
       </c>
       <c r="O31" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="P31" s="18">
         <v>1</v>
@@ -5246,7 +5113,7 @@
         <v>1</v>
       </c>
       <c r="U31" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="V31" s="18">
         <v>1</v>
@@ -5261,7 +5128,7 @@
         <v>1</v>
       </c>
       <c r="Z31" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AA31" s="18">
         <v>1</v>
@@ -5270,28 +5137,28 @@
         <v>1</v>
       </c>
       <c r="AC31" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AD31" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AE31" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AF31" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AG31" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AH31" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AI31" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AJ31" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AK31" s="5" t="s">
         <v>3</v>
@@ -5301,7 +5168,7 @@
       </c>
       <c r="AM31" s="5"/>
     </row>
-    <row r="32" spans="1:39" s="4" customFormat="1">
+    <row r="32" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>19</v>
       </c>
@@ -5312,7 +5179,7 @@
         <v>2</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E32" s="14">
         <v>133</v>
@@ -5416,7 +5283,7 @@
       </c>
       <c r="AM32" s="1"/>
     </row>
-    <row r="33" spans="1:39" s="7" customFormat="1">
+    <row r="33" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>19</v>
       </c>
@@ -5427,7 +5294,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="1">
@@ -5529,7 +5396,7 @@
       </c>
       <c r="AM33" s="1"/>
     </row>
-    <row r="34" spans="1:39">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>20</v>
       </c>
@@ -5540,7 +5407,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E34" s="14"/>
       <c r="F34" s="1">
@@ -5646,18 +5513,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:39">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>21</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="1">
@@ -5668,7 +5535,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J35" s="15">
         <v>1</v>
@@ -5716,28 +5583,28 @@
         <v>0</v>
       </c>
       <c r="Y35" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Z35" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AA35" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AB35" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AC35" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AD35" s="15">
         <v>0</v>
       </c>
       <c r="AE35" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AF35" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AG35" s="15">
         <v>0</v>
@@ -5759,7 +5626,7 @@
       </c>
       <c r="AM35" s="1"/>
     </row>
-    <row r="36" spans="1:39">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>22</v>
       </c>
@@ -5770,7 +5637,7 @@
         <v>2</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E36" s="14"/>
       <c r="F36" s="1">
@@ -5874,18 +5741,18 @@
       </c>
       <c r="AM36" s="1"/>
     </row>
-    <row r="37" spans="1:39">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>23</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E37" s="17"/>
       <c r="F37" s="5">
@@ -5978,16 +5845,16 @@
         <v>0</v>
       </c>
       <c r="AK37" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AL37" s="19">
         <v>42530</v>
       </c>
       <c r="AM37" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:39">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>24</v>
       </c>
@@ -5995,10 +5862,10 @@
         <v>36</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E38" s="23">
         <v>130</v>
@@ -6013,7 +5880,7 @@
         <v>1</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J38" s="18">
         <v>1</v>
@@ -6022,16 +5889,16 @@
         <v>1</v>
       </c>
       <c r="L38" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M38" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="N38" s="18">
         <v>1</v>
       </c>
       <c r="O38" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="P38" s="18">
         <v>1</v>
@@ -6043,13 +5910,13 @@
         <v>1</v>
       </c>
       <c r="S38" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="T38" s="18">
         <v>1</v>
       </c>
       <c r="U38" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="V38" s="18">
         <v>1</v>
@@ -6082,19 +5949,19 @@
         <v>1</v>
       </c>
       <c r="AF38" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AG38" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AH38" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AI38" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AJ38" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AK38" s="5" t="s">
         <v>37</v>
@@ -6106,7 +5973,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:39" s="4" customFormat="1">
+    <row r="39" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>25</v>
       </c>
@@ -6117,7 +5984,7 @@
         <v>2</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="1">
@@ -6223,7 +6090,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:39" s="4" customFormat="1">
+    <row r="40" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>26</v>
       </c>
@@ -6234,7 +6101,7 @@
         <v>2</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E40" s="14"/>
       <c r="F40" s="1">
@@ -6268,10 +6135,10 @@
         <v>1</v>
       </c>
       <c r="P40" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Q40" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="R40" s="15">
         <v>0</v>
@@ -6286,10 +6153,10 @@
         <v>0</v>
       </c>
       <c r="V40" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="W40" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="X40" s="15">
         <v>1</v>
@@ -6316,7 +6183,7 @@
         <v>1</v>
       </c>
       <c r="AF40" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AG40" s="15">
         <v>0</v>
@@ -6340,18 +6207,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:39">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>27</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E41" s="14">
         <v>93</v>
@@ -6456,10 +6323,10 @@
         <v>42530</v>
       </c>
       <c r="AM41" s="15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:39">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>28</v>
       </c>
@@ -6470,7 +6337,7 @@
         <v>2</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="1">
@@ -6574,7 +6441,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:39">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>31</v>
       </c>
@@ -6585,7 +6452,7 @@
         <v>2</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E43" s="14"/>
       <c r="F43" s="1">
@@ -6596,61 +6463,61 @@
         <v>0</v>
       </c>
       <c r="J43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="N43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="O43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="P43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Q43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="R43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="S43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="T43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="U43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="V43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="W43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="X43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Y43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Z43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AA43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AB43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AC43" s="15">
         <v>1</v>
@@ -6662,19 +6529,19 @@
         <v>1</v>
       </c>
       <c r="AF43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AG43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AH43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AI43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AJ43" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AK43" s="1" t="s">
         <v>9</v>
@@ -6684,18 +6551,18 @@
       </c>
       <c r="AM43" s="1"/>
     </row>
-    <row r="44" spans="1:39">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>34</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E44" s="20"/>
       <c r="F44" s="8">
@@ -6765,7 +6632,7 @@
         <v>0</v>
       </c>
       <c r="AB44" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AC44" s="21">
         <v>1</v>
@@ -6798,21 +6665,21 @@
         <v>42163</v>
       </c>
       <c r="AM44" s="8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
-    <row r="45" spans="1:39" s="7" customFormat="1">
+    <row r="45" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>35</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E45" s="17">
         <v>200</v>
@@ -6909,25 +6776,25 @@
         <v>0</v>
       </c>
       <c r="AK45" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AL45" s="29">
         <v>42530</v>
       </c>
       <c r="AM45" s="18"/>
     </row>
-    <row r="46" spans="1:39">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>35</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E46" s="17"/>
       <c r="F46" s="5">
@@ -7022,25 +6889,25 @@
         <v>0</v>
       </c>
       <c r="AK46" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AL46" s="29">
         <v>42530</v>
       </c>
       <c r="AM46" s="18"/>
     </row>
-    <row r="47" spans="1:39" s="7" customFormat="1">
+    <row r="47" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>36</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E47" s="14">
         <v>131</v>
@@ -7137,27 +7004,27 @@
         <v>0</v>
       </c>
       <c r="AK47" s="15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="AL47" s="15">
         <v>42530</v>
       </c>
       <c r="AM47" s="15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:39">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>36</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="1">
@@ -7252,16 +7119,16 @@
         <v>0</v>
       </c>
       <c r="AK48" s="15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="AL48" s="15">
         <v>42530</v>
       </c>
       <c r="AM48" s="15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
-    <row r="49" spans="1:39">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>37</v>
       </c>
@@ -7272,7 +7139,7 @@
         <v>2</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E49" s="14"/>
       <c r="F49" s="1">
@@ -7374,18 +7241,18 @@
       </c>
       <c r="AM49" s="1"/>
     </row>
-    <row r="50" spans="1:39">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>38</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E50" s="14">
         <v>140</v>
@@ -7482,25 +7349,25 @@
         <v>1</v>
       </c>
       <c r="AK50" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="AL50" s="16">
         <v>42530</v>
       </c>
       <c r="AM50" s="1"/>
     </row>
-    <row r="51" spans="1:39">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>38</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E51" s="14"/>
       <c r="F51" s="1">
@@ -7595,14 +7462,14 @@
         <v>1</v>
       </c>
       <c r="AK51" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="AL51" s="16">
         <v>42530</v>
       </c>
       <c r="AM51" s="1"/>
     </row>
-    <row r="52" spans="1:39" s="7" customFormat="1">
+    <row r="52" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>39</v>
       </c>
@@ -7613,7 +7480,7 @@
         <v>2</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E52" s="14">
         <v>180</v>
@@ -7719,7 +7586,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:39">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>39</v>
       </c>
@@ -7730,7 +7597,7 @@
         <v>2</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E53" s="14"/>
       <c r="F53" s="1">
@@ -7834,7 +7701,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:39">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>39</v>
       </c>
@@ -7845,7 +7712,7 @@
         <v>2</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E54" s="14"/>
       <c r="F54" s="1">
@@ -7949,7 +7816,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:39">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>40</v>
       </c>
@@ -7960,7 +7827,7 @@
         <v>2</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E55" s="14">
         <v>100</v>
@@ -8036,7 +7903,7 @@
         <v>1</v>
       </c>
       <c r="AE55" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AF55" s="15">
         <v>1</v>
@@ -8061,18 +7928,18 @@
       </c>
       <c r="AM55" s="1"/>
     </row>
-    <row r="56" spans="1:39" s="4" customFormat="1">
+    <row r="56" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>41</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>98</v>
+        <v>171</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E56" s="17"/>
       <c r="F56" s="5">
@@ -8088,34 +7955,34 @@
         <v>30</v>
       </c>
       <c r="J56" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K56" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L56" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M56" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="N56" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="O56" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="P56" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Q56" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="R56" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="S56" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="T56" s="18">
         <v>1</v>
@@ -8176,18 +8043,18 @@
       </c>
       <c r="AM56" s="5"/>
     </row>
-    <row r="57" spans="1:39" s="4" customFormat="1">
+    <row r="57" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>42</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E57" s="17">
         <v>136</v>
@@ -8291,18 +8158,18 @@
       </c>
       <c r="AM57" s="5"/>
     </row>
-    <row r="58" spans="1:39">
+    <row r="58" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>42</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E58" s="17"/>
       <c r="F58" s="5">
@@ -8404,18 +8271,18 @@
       </c>
       <c r="AM58" s="5"/>
     </row>
-    <row r="59" spans="1:39">
+    <row r="59" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>43</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E59" s="14"/>
       <c r="F59" s="1">
@@ -8429,64 +8296,64 @@
         <v>50</v>
       </c>
       <c r="J59" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K59" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L59" s="15">
         <v>1</v>
       </c>
       <c r="M59" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="N59" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="O59" s="15">
         <v>0</v>
       </c>
       <c r="P59" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Q59" s="15">
         <v>0</v>
       </c>
       <c r="R59" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="S59" s="15">
         <v>0</v>
       </c>
       <c r="T59" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="U59" s="15">
         <v>0</v>
       </c>
       <c r="V59" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="W59" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="X59" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Y59" s="15">
         <v>0</v>
       </c>
       <c r="Z59" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AA59" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AB59" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AC59" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AD59" s="15">
         <v>0</v>
@@ -8498,10 +8365,10 @@
         <v>0</v>
       </c>
       <c r="AG59" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AH59" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AI59" s="15">
         <v>0</v>
@@ -8510,14 +8377,14 @@
         <v>0</v>
       </c>
       <c r="AK59" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AL59" s="16">
         <v>42524</v>
       </c>
       <c r="AM59" s="1"/>
     </row>
-    <row r="60" spans="1:39">
+    <row r="60" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>45</v>
       </c>
@@ -8528,7 +8395,7 @@
         <v>2</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E60" s="20"/>
       <c r="F60" s="8">
@@ -8630,7 +8497,7 @@
       </c>
       <c r="AM60" s="8"/>
     </row>
-    <row r="61" spans="1:39">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>46</v>
       </c>
@@ -8641,7 +8508,7 @@
         <v>2</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E61" s="14"/>
       <c r="F61" s="1">
@@ -8655,73 +8522,73 @@
         <v>50</v>
       </c>
       <c r="J61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M61" s="24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="N61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="O61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="P61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Q61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="R61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="S61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="T61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="U61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="V61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="W61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="X61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Y61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Z61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AA61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AB61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AC61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AD61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AE61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AF61" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AG61" s="15">
         <v>1</v>
@@ -8745,7 +8612,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="1:39">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>47</v>
       </c>
@@ -8756,7 +8623,7 @@
         <v>2</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E62" s="14"/>
       <c r="F62" s="1">
@@ -8857,21 +8724,21 @@
         <v>42531</v>
       </c>
       <c r="AM62" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
-    <row r="63" spans="1:39" ht="15" thickBot="1">
+    <row r="63" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>49</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E63" s="14"/>
       <c r="F63" s="1">
@@ -8969,7 +8836,7 @@
         <v>42530</v>
       </c>
       <c r="AM63" s="26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>